<commit_message>
Fix test data in credentials.xlsx, add comments in FrameworkUtils, Add Test Case desc in TestClass
</commit_message>
<xml_diff>
--- a/src/main/resources/credentials.xlsx
+++ b/src/main/resources/credentials.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SUKHPREET KAUR\IdeaProjects\seleniumFinalProject\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SUKHPREET KAUR\Downloads\seleniumPractice\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3CB4FC9-FAAB-4525-AC46-6C09875FCED8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B868B92-8FFA-4D52-91BF-53EDE4CA3BD1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{66C97393-BBE1-482C-961A-2633376B9A80}"/>
   </bookViews>
@@ -428,7 +428,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>